<commit_message>
added logic for category lables in the bottom left box
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,33 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>chik</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>$23.67</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>6/10/24</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>